<commit_message>
Added additional sheets in the ExcelData file.
</commit_message>
<xml_diff>
--- a/Data Files/API-Phase2-RESTAssuredCucumber-Data.xlsx
+++ b/Data Files/API-Phase2-RESTAssuredCucumber-Data.xlsx
@@ -5,15 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arunm\Contacts\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arunm\Contacts\Desktop\July23-API-Phase2-RESTAssuredHackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70049338-57C0-417B-8CA1-3152309920C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428C7CB9-62A0-45B9-AA56-AEEA8B9019CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0E9CFF59-B40C-4859-8CD1-E76179D2975D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="6" xr2:uid="{0E9CFF59-B40C-4859-8CD1-E76179D2975D}"/>
   </bookViews>
   <sheets>
     <sheet name="ProgramPOSTValidData" sheetId="1" r:id="rId1"/>
+    <sheet name="ProgramPOSTInvalidData" sheetId="2" r:id="rId2"/>
+    <sheet name="ProgramPOSTNoProgramName" sheetId="5" r:id="rId3"/>
+    <sheet name="ProgramPOSTNoProgramDescription" sheetId="3" r:id="rId4"/>
+    <sheet name="ProgramPOSTNoProgramStatus" sheetId="4" r:id="rId5"/>
+    <sheet name="ProgramGETValidProgramId" sheetId="6" r:id="rId6"/>
+    <sheet name="ProgramGETInvalidProgramId" sheetId="7" r:id="rId7"/>
+    <sheet name="ProgramDELETEProgramById" sheetId="8" r:id="rId8"/>
+    <sheet name="ProgramDELETEByName" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet9" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
   <si>
     <t>programName</t>
   </si>
@@ -46,13 +55,25 @@
   </si>
   <si>
     <t>API Testing</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDE-088</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-015</t>
+  </si>
+  <si>
+    <t>programId</t>
+  </si>
+  <si>
+    <t>90*0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,13 +81,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFE"/>
+        <bgColor rgb="FFFFFFFE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -93,15 +139,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{30E9D335-A864-4EFB-9257-F53F70725839}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{AA7A26E4-3420-423D-BCC6-756FEF86F530}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -415,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E4E36E-8861-4F96-85B4-48415530EA86}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,7 +506,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -462,4 +518,239 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B10F50-9531-4154-B5C6-8E70F9D0F6BD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6AE954-3042-4D15-AAB0-553D14FF33EA}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5BA1C8-ECAA-4C8B-8E50-DE75B43F80C8}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249E5685-5468-4093-A839-2485C97D9AF3}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD9C371-64AD-485D-BC9B-1790CF7CC473}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5593D41-99AF-4E19-A7B0-35749D27D8E1}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>10857</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A36F2FC-005D-4DA9-AC54-5A52FF081A2F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46C1994-431C-45CD-ACFA-BD70DE570B22}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63A806C-571E-4010-B6F8-E6E299A72141}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Additional Sheets are added in Excel Data Sheet.
</commit_message>
<xml_diff>
--- a/Data Files/API-Phase2-RESTAssuredCucumber-Data.xlsx
+++ b/Data Files/API-Phase2-RESTAssuredCucumber-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arunm\Contacts\Desktop\July23-API-Phase2-RESTAssuredHackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428C7CB9-62A0-45B9-AA56-AEEA8B9019CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920F53E6-95D3-405C-AC27-8AB36B5232F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="6" xr2:uid="{0E9CFF59-B40C-4859-8CD1-E76179D2975D}"/>
   </bookViews>
@@ -66,7 +66,7 @@
     <t>programId</t>
   </si>
   <si>
-    <t>90*0</t>
+    <t>90*1</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Program Module- POST Request- Completed
</commit_message>
<xml_diff>
--- a/Data Files/API-Phase2-RESTAssuredCucumber-Data.xlsx
+++ b/Data Files/API-Phase2-RESTAssuredCucumber-Data.xlsx
@@ -5,24 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arunm\Contacts\Desktop\July23-API-Phase2-RESTAssuredHackathon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Preet\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920F53E6-95D3-405C-AC27-8AB36B5232F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4DB32F-2EA3-46A3-9582-1C6B17A620CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="6" xr2:uid="{0E9CFF59-B40C-4859-8CD1-E76179D2975D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="1" xr2:uid="{0E9CFF59-B40C-4859-8CD1-E76179D2975D}"/>
   </bookViews>
   <sheets>
     <sheet name="ProgramPOSTValidData" sheetId="1" r:id="rId1"/>
-    <sheet name="ProgramPOSTInvalidData" sheetId="2" r:id="rId2"/>
-    <sheet name="ProgramPOSTNoProgramName" sheetId="5" r:id="rId3"/>
-    <sheet name="ProgramPOSTNoProgramDescription" sheetId="3" r:id="rId4"/>
-    <sheet name="ProgramPOSTNoProgramStatus" sheetId="4" r:id="rId5"/>
-    <sheet name="ProgramGETValidProgramId" sheetId="6" r:id="rId6"/>
-    <sheet name="ProgramGETInvalidProgramId" sheetId="7" r:id="rId7"/>
-    <sheet name="ProgramDELETEProgramById" sheetId="8" r:id="rId8"/>
-    <sheet name="ProgramDELETEByName" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet9" sheetId="10" r:id="rId10"/>
+    <sheet name="ProgramPOSTNoProgramName" sheetId="5" r:id="rId2"/>
+    <sheet name="ProgramPOSTNOProgramDescription" sheetId="3" r:id="rId3"/>
+    <sheet name="ProgramPOSTNoProgramStatus" sheetId="4" r:id="rId4"/>
+    <sheet name="ProgramGETValidProgramId" sheetId="6" r:id="rId5"/>
+    <sheet name="ProgramGETInvalidProgramId" sheetId="7" r:id="rId6"/>
+    <sheet name="ProgramDELETEProgramById" sheetId="8" r:id="rId7"/>
+    <sheet name="ProgramDELETEByName" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="22">
   <si>
     <t>programName</t>
   </si>
@@ -45,9 +44,6 @@
     <t>programStatus</t>
   </si>
   <si>
-    <t>July23-AssuredNinjas-SDET-014</t>
-  </si>
-  <si>
     <t>Selenium</t>
   </si>
   <si>
@@ -60,13 +56,49 @@
     <t>July23-AssuredNinjas-SDE-088</t>
   </si>
   <si>
-    <t>July23-AssuredNinjas-SDET-015</t>
-  </si>
-  <si>
     <t>programId</t>
   </si>
   <si>
     <t>90*1</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDE-090</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-515</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-516</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-517</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-518</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-519</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-520</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-521</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-522</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-523</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-524</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-525</t>
+  </si>
+  <si>
+    <t>July23-AssuredNinjas-SDET-526</t>
   </si>
 </sst>
 </file>
@@ -144,11 +176,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -469,50 +500,278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E4E36E-8861-4F96-85B4-48415530EA86}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5BA1C8-ECAA-4C8B-8E50-DE75B43F80C8}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249E5685-5468-4093-A839-2485C97D9AF3}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD9C371-64AD-485D-BC9B-1790CF7CC473}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -520,7 +779,91 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5593D41-99AF-4E19-A7B0-35749D27D8E1}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10857</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A36F2FC-005D-4DA9-AC54-5A52FF081A2F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46C1994-431C-45CD-ACFA-BD70DE570B22}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63A806C-571E-4010-B6F8-E6E299A72141}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B10F50-9531-4154-B5C6-8E70F9D0F6BD}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -528,228 +871,7 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6AE954-3042-4D15-AAB0-553D14FF33EA}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="33.109375" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE5BA1C8-ECAA-4C8B-8E50-DE75B43F80C8}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249E5685-5468-4093-A839-2485C97D9AF3}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD9C371-64AD-485D-BC9B-1790CF7CC473}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5593D41-99AF-4E19-A7B0-35749D27D8E1}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>10857</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A36F2FC-005D-4DA9-AC54-5A52FF081A2F}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46C1994-431C-45CD-ACFA-BD70DE570B22}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63A806C-571E-4010-B6F8-E6E299A72141}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ahila final project updates
</commit_message>
<xml_diff>
--- a/Data Files/API-Phase2-RESTAssuredCucumber-Data.xlsx
+++ b/Data Files/API-Phase2-RESTAssuredCucumber-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ahila\git\API.Phase2.RestAssuredCucumber\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229DB5F3-74E3-44B9-8B2F-7262BE5C928C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491342A2-AB5B-42FD-B974-E5595B8BCA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="10" xr2:uid="{0E9CFF59-B40C-4859-8CD1-E76179D2975D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="7" activeTab="12" xr2:uid="{0E9CFF59-B40C-4859-8CD1-E76179D2975D}"/>
   </bookViews>
   <sheets>
     <sheet name="ProgramPOSTValidData" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,8 @@
     <sheet name="Sheet9" sheetId="10" r:id="rId9"/>
     <sheet name="BatchDeleteByInvalidId" sheetId="11" r:id="rId10"/>
     <sheet name="BatchDeleteByValidId" sheetId="12" r:id="rId11"/>
+    <sheet name="UserDeleteByUserId" sheetId="13" r:id="rId12"/>
+    <sheet name="UserDeleteByInvalidUserId" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>programName</t>
   </si>
@@ -107,13 +109,22 @@
   </si>
   <si>
     <t>BatchId</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>U123454</t>
+  </si>
+  <si>
+    <t>U132@</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +147,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,12 +198,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -192,8 +212,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{30E9D335-A864-4EFB-9257-F53F70725839}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{AA7A26E4-3420-423D-BCC6-756FEF86F530}"/>
@@ -514,14 +536,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -543,7 +565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -554,7 +576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -565,7 +587,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -576,7 +598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -587,7 +609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -598,7 +620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -609,7 +631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -620,7 +642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -631,7 +653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -642,7 +664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -653,7 +675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -677,14 +699,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -699,23 +721,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D289D19-F417-4665-A92E-E69C91000EDC}">
   <dimension ref="A1:A2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6484</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4720F70B-0AF2-4F7D-9B8F-05D88BE2407C}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0732117B-6F53-48D4-B19B-B5AFC5BF39EE}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>6484</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5CF9823F-1BB8-47DF-9E6C-C245A050298C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -728,14 +803,14 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -767,14 +842,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -785,7 +860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -807,14 +882,14 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -825,7 +900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -846,14 +921,14 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10857</v>
       </c>
@@ -871,14 +946,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -896,9 +971,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -916,7 +991,7 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -930,7 +1005,7 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>